<commit_message>
chore: re-measured values with higher precision
</commit_message>
<xml_diff>
--- a/results/bmark_combined.xlsx
+++ b/results/bmark_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\root\projects\hash_functions\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6D8893-6626-482E-8B7E-9DC8035BF6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66454C3-6D59-441B-9F99-9E114CAE7409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>test_id</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>deviation</t>
-  </si>
-  <si>
-    <t>bmark_2</t>
   </si>
   <si>
     <t>rel. error</t>
@@ -116,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -124,110 +121,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,13 +443,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>250000</v>
+        <v>4031250</v>
       </c>
       <c r="C2">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D2">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -553,13 +457,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>250000</v>
+        <v>4000000</v>
       </c>
       <c r="C3">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D3">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -567,13 +471,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>265625</v>
+        <v>3984375</v>
       </c>
       <c r="C4">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D4">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,13 +485,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>250000</v>
+        <v>4031250</v>
       </c>
       <c r="C5">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D5">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -595,13 +499,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>250000</v>
+        <v>4000000</v>
       </c>
       <c r="C6">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D6">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -609,13 +513,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>250000</v>
+        <v>4015625</v>
       </c>
       <c r="C7">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
       <c r="D7">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -623,13 +527,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>250000</v>
+        <v>3968750</v>
       </c>
       <c r="C8">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D8">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -637,13 +541,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>234375</v>
+        <v>4000000</v>
       </c>
       <c r="C9">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D9">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -651,13 +555,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>265625</v>
+        <v>3984375</v>
       </c>
       <c r="C10">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
       <c r="D10">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,13 +569,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>250000</v>
+        <v>3984375</v>
       </c>
       <c r="C11">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D11">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -679,13 +583,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>250000</v>
+        <v>3968750</v>
       </c>
       <c r="C12">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D12">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -693,13 +597,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>234375</v>
+        <v>3984375</v>
       </c>
       <c r="C13">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D13">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,13 +611,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>265625</v>
+        <v>3968750</v>
       </c>
       <c r="C14">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
       <c r="D14">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -721,13 +625,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>234375</v>
+        <v>3968750</v>
       </c>
       <c r="C15">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D15">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -735,13 +639,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>265625</v>
+        <v>3968750</v>
       </c>
       <c r="C16">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
       <c r="D16">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -749,13 +653,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>250000</v>
+        <v>4000000</v>
       </c>
       <c r="C17">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D17">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -763,13 +667,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>234375</v>
+        <v>4046875</v>
       </c>
       <c r="C18">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
       <c r="D18">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -777,13 +681,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>265625</v>
+        <v>4125000</v>
       </c>
       <c r="C19">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D19">
-        <v>78125</v>
+        <v>1343750</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -791,13 +695,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>250000</v>
+        <v>4031250</v>
       </c>
       <c r="C20">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D20">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -805,13 +709,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>250000</v>
+        <v>4046875</v>
       </c>
       <c r="C21">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D21">
-        <v>93750</v>
+        <v>1343750</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -819,13 +723,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>250000</v>
+        <v>4031250</v>
       </c>
       <c r="C22">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D22">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,13 +737,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>250000</v>
+        <v>4000000</v>
       </c>
       <c r="C23">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D23">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -847,13 +751,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>250000</v>
+        <v>4000000</v>
       </c>
       <c r="C24">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
       <c r="D24">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -861,13 +765,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>250000</v>
+        <v>4015625</v>
       </c>
       <c r="C25">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D25">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -875,13 +779,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>250000</v>
+        <v>4015625</v>
       </c>
       <c r="C26">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D26">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -889,13 +793,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>250000</v>
+        <v>4015625</v>
       </c>
       <c r="C27">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D27">
-        <v>78125</v>
+        <v>1343750</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -903,13 +807,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>250000</v>
+        <v>4046875</v>
       </c>
       <c r="C28">
-        <v>78125</v>
+        <v>1375000</v>
       </c>
       <c r="D28">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,13 +821,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>265625</v>
+        <v>4171875</v>
       </c>
       <c r="C29">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D29">
-        <v>93750</v>
+        <v>1343750</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -931,13 +835,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>234375</v>
+        <v>4156250</v>
       </c>
       <c r="C30">
-        <v>78125</v>
+        <v>1390625</v>
       </c>
       <c r="D30">
-        <v>78125</v>
+        <v>1343750</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -945,13 +849,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>250000</v>
+        <v>4015625</v>
       </c>
       <c r="C31">
-        <v>93750</v>
+        <v>1375000</v>
       </c>
       <c r="D31">
-        <v>93750</v>
+        <v>1390625</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -959,13 +863,13 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>265625</v>
+        <v>4062500</v>
       </c>
       <c r="C32">
-        <v>78125</v>
+        <v>1390625</v>
       </c>
       <c r="D32">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -973,13 +877,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>250000</v>
+        <v>4062500</v>
       </c>
       <c r="C33">
-        <v>93750</v>
+        <v>1359375</v>
       </c>
       <c r="D33">
-        <v>78125</v>
+        <v>1359375</v>
       </c>
     </row>
   </sheetData>
@@ -991,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2184DC31-09BE-47B9-80E0-FCA191440139}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,251 +908,254 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>6</v>
+      <c r="B1" s="1" t="str">
+        <f>Results!B1</f>
+        <v>bmark_0</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f>Results!C1</f>
+        <v>bmark_1</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f>Results!D1</f>
+        <v>time_2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14">
-        <f>AVERAGE(Results!B2:B33)</f>
-        <v>250976.5625</v>
+      <c r="B2" s="2">
+        <f>AVERAGE(Results!B:B)</f>
+        <v>4021972.65625</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(Results!C2:C33)</f>
-        <v>85937.5</v>
-      </c>
-      <c r="D2" s="3">
-        <f>AVERAGE(Results!D2:D33)</f>
-        <v>83984.375</v>
+        <f>AVERAGE(Results!C:C)</f>
+        <v>1372558.59375</v>
+      </c>
+      <c r="D2" s="2">
+        <f>AVERAGE(Results!D:D)</f>
+        <v>1360839.84375</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15">
-        <f>_xlfn.STDEV.S(Results!B2:B33)</f>
-        <v>9670.6571846521638</v>
-      </c>
-      <c r="C3" s="5">
-        <f>_xlfn.STDEV.S(Results!C2:C33)</f>
-        <v>7937.5079375119067</v>
-      </c>
-      <c r="D3" s="6">
-        <f>_xlfn.STDEV.S(Results!D2:D33)</f>
-        <v>7685.4590130931983</v>
+      <c r="B3" s="2">
+        <f>_xlfn.STDEV.S(Results!B:B)</f>
+        <v>50647.79688206641</v>
+      </c>
+      <c r="C3" s="2">
+        <f>_xlfn.STDEV.S(Results!C:C)</f>
+        <v>8045.2966859601247</v>
+      </c>
+      <c r="D3" s="2">
+        <f>_xlfn.STDEV.S(Results!D:D)</f>
+        <v>10766.502448557674</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
         <f>B3/B2</f>
-        <v>3.8532112673477885E-2</v>
-      </c>
-      <c r="C4" s="10">
+        <v>1.2592775041213065E-2</v>
+      </c>
+      <c r="C4" s="3">
         <f t="shared" ref="C4:D4" si="0">C3/C2</f>
-        <v>9.2363728727411276E-2</v>
-      </c>
-      <c r="D4" s="11">
+        <v>5.8615324129656123E-3</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>9.151058173729576E-2</v>
+        <v>7.9116602133642334E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="14">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
         <f>$B2/B2</f>
         <v>1</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:D5" si="1">$B2/C2</f>
-        <v>2.9204545454545454</v>
-      </c>
-      <c r="D5" s="3">
+        <v>2.9302739238705087</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>2.9883720930232558</v>
+        <v>2.9555077143882311</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <f>B5*(1+$B4)/(1-B4)</f>
+        <v>1.0255067508580133</v>
+      </c>
+      <c r="C6" s="2">
+        <f>C5*(1+$B4)/(1-C4)</f>
+        <v>2.9846689379245595</v>
+      </c>
+      <c r="D6" s="2">
+        <f>D5*(1+$B4)/(1-D4)</f>
+        <v>3.016592009146811</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="15">
-        <f>B5*(1+$B4)/(1-B4)</f>
-        <v>1.0801526773413537</v>
-      </c>
-      <c r="C6" s="5">
-        <f>C5*(1+$B4)/(1-C4)</f>
-        <v>3.3416313616524471</v>
-      </c>
-      <c r="D6" s="6">
-        <f>D5*(1+$B4)/(1-D4)</f>
-        <v>3.4161326712607591</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="2">
+        <f>B5*(1-$B4)/(1+B4)</f>
+        <v>0.9751276616788016</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:D7" si="2">C5*(1-$B4)/(1+C4)</f>
+        <v>2.8765128701135914</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8953823889591668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="15">
-        <f>B5*(1-$B4)/(1+B4)</f>
-        <v>0.92579504821611103</v>
-      </c>
-      <c r="C7" s="5">
-        <f t="shared" ref="C7:D7" si="2">C5*(1-$B4)/(1+C4)</f>
-        <v>2.570502102923641</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" si="2"/>
-        <v>2.6323371031836071</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="2">
+        <f>AVERAGE(B6:B7)</f>
+        <v>1.0003172062684076</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:D8" si="3">AVERAGE(C6:C7)</f>
+        <v>2.9305909040190752</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="3"/>
+        <v>2.9559871990529887</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15">
-        <f>AVERAGE(B6:B7)</f>
-        <v>1.0029738627787324</v>
-      </c>
-      <c r="C8" s="5">
-        <f t="shared" ref="C8:D8" si="3">AVERAGE(C6:C7)</f>
-        <v>2.9560667322880443</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" si="3"/>
-        <v>3.0242348872221831</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="15">
+      <c r="B9" s="2">
         <f>(B6-B7)/2</f>
-        <v>7.7178814562621323E-2</v>
-      </c>
-      <c r="C9" s="5">
+        <v>2.5189544589605872E-2</v>
+      </c>
+      <c r="C9" s="2">
         <f t="shared" ref="C9:D9" si="4">(C6-C7)/2</f>
-        <v>0.38556462936440306</v>
-      </c>
-      <c r="D9" s="6">
+        <v>5.4078033905484046E-2</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="4"/>
-        <v>0.391897784038576</v>
+        <v>6.0604810093822126E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="17">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4">
         <f>B9/B8</f>
-        <v>7.694997589348733E-2</v>
-      </c>
-      <c r="C10" s="8">
-        <f t="shared" ref="C10:D10" si="5">C9/C8</f>
-        <v>0.1304316391619379</v>
-      </c>
-      <c r="D10" s="9">
+        <v>2.5181556841927352E-2</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" ref="C10" si="5">C9/C8</f>
+        <v>1.8452945387676004E-2</v>
+      </c>
+      <c r="D10" s="4">
         <f>D9/D8</f>
-        <v>0.12958576256573162</v>
+        <v>2.0502392606178445E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2">
         <f>B2/C2</f>
-        <v>2.9204545454545454</v>
-      </c>
-      <c r="D11" s="3">
+        <v>2.9302739238705087</v>
+      </c>
+      <c r="D11" s="2">
         <f>C2/D2</f>
-        <v>1.0232558139534884</v>
+        <v>1.0086114101184069</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="5">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
         <f>C11*(1+C4)/(1-B4)</f>
-        <v>3.3180500970473155</v>
-      </c>
-      <c r="D12" s="6">
+        <v>2.9850397535597999</v>
+      </c>
+      <c r="D12" s="2">
         <f>D11*(1+D4)/(1-C4)</f>
-        <v>1.2305530134758214</v>
+        <v>1.0225851166890751</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
+        <f>C11*(1-C4)/(1+B4)</f>
+        <v>2.8768702484256901</v>
+      </c>
+      <c r="D13" s="2">
+        <f>D11*(1-D4)/(1+C4)</f>
+        <v>0.99480056360621372</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="5">
-        <f>C11*(1-C4)/(1+B4)</f>
-        <v>2.5523625525972058</v>
-      </c>
-      <c r="D13" s="6">
-        <f>D11*(1-D4)/(1+C4)</f>
-        <v>0.85101423152847244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
+        <f>AVERAGE(C12:C13)</f>
+        <v>2.930955000992745</v>
+      </c>
+      <c r="D14" s="2">
+        <f>AVERAGE(D12:D13)</f>
+        <v>1.0086928401476445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="5">
-        <f>AVERAGE(C12:C13)</f>
-        <v>2.9352063248222606</v>
-      </c>
-      <c r="D14" s="6">
-        <f>AVERAGE(D12:D13)</f>
-        <v>1.040783622502147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
+        <f>(C12-C13)/2</f>
+        <v>5.4084752567054917E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <f>(D12-D13)/2</f>
+        <v>1.3892276541430715E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="5">
-        <f>(C12-C13)/2</f>
-        <v>0.38284377222505483</v>
-      </c>
-      <c r="D15" s="6">
-        <f>(D12-D13)/2</f>
-        <v>0.18976939097367446</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="8">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4">
         <f>C15/C14</f>
-        <v>0.13043163916193784</v>
-      </c>
-      <c r="D16" s="9">
+        <v>1.845294538767598E-2</v>
+      </c>
+      <c r="D16" s="4">
         <f>D15/D14</f>
-        <v>0.18233318325806283</v>
+        <v>1.3772553931677827E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: article rewrite fix: check if the table is NULL in ctor
</commit_message>
<xml_diff>
--- a/results/bmark_combined.xlsx
+++ b/results/bmark_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\root\projects\hash_functions\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66454C3-6D59-441B-9F99-9E114CAE7409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CF15FB-B096-45C0-9C3E-AF60C1FDB8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4788" yWindow="1008" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -126,12 +126,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,265 +894,245 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2184DC31-09BE-47B9-80E0-FCA191440139}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <f>Results!B1</f>
         <v>bmark_0</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <f>Results!C1</f>
         <v>bmark_1</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <f>Results!D1</f>
         <v>time_2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <f>AVERAGE(Results!B:B)</f>
-        <v>4021972.65625</v>
-      </c>
-      <c r="C2" s="2">
-        <f>AVERAGE(Results!C:C)</f>
-        <v>1372558.59375</v>
-      </c>
-      <c r="D2" s="2">
-        <f>AVERAGE(Results!D:D)</f>
-        <v>1360839.84375</v>
+      <c r="B2" s="1">
+        <f>AVERAGE(Results!B:B)/1000000</f>
+        <v>4.02197265625</v>
+      </c>
+      <c r="C2" s="1">
+        <f>AVERAGE(Results!C:C)/1000000</f>
+        <v>1.37255859375</v>
+      </c>
+      <c r="D2" s="1">
+        <f>AVERAGE(Results!D:D)/1000000</f>
+        <v>1.36083984375</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
-        <f>_xlfn.STDEV.S(Results!B:B)</f>
-        <v>50647.79688206641</v>
-      </c>
-      <c r="C3" s="2">
-        <f>_xlfn.STDEV.S(Results!C:C)</f>
-        <v>8045.2966859601247</v>
-      </c>
-      <c r="D3" s="2">
-        <f>_xlfn.STDEV.S(Results!D:D)</f>
-        <v>10766.502448557674</v>
+      <c r="B3" s="1">
+        <f>_xlfn.STDEV.S(Results!B:B)/1000000</f>
+        <v>5.0647796882066408E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <f>_xlfn.STDEV.S(Results!C:C)/1000000</f>
+        <v>8.0452966859601242E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <f>_xlfn.STDEV.S(Results!D:D)/1000000</f>
+        <v>1.0766502448557674E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <f>B3/B2</f>
-        <v>1.2592775041213065E-2</v>
-      </c>
-      <c r="C4" s="3">
+        <v>1.2592775041213063E-2</v>
+      </c>
+      <c r="C4" s="2">
         <f t="shared" ref="C4:D4" si="0">C3/C2</f>
-        <v>5.8615324129656123E-3</v>
-      </c>
-      <c r="D4" s="3">
+        <v>5.8615324129656114E-3</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>7.9116602133642334E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <f>$B2/B2</f>
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
         <f t="shared" ref="C5:D5" si="1">$B2/C2</f>
         <v>2.9302739238705087</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>2.9555077143882311</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2">
-        <f>B5*(1+$B4)/(1-B4)</f>
-        <v>1.0255067508580133</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
         <f>C5*(1+$B4)/(1-C4)</f>
         <v>2.9846689379245595</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f>D5*(1+$B4)/(1-D4)</f>
         <v>3.016592009146811</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
-        <f>B5*(1-$B4)/(1+B4)</f>
-        <v>0.9751276616788016</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
         <f t="shared" ref="C7:D7" si="2">C5*(1-$B4)/(1+C4)</f>
         <v>2.8765128701135914</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <f t="shared" si="2"/>
         <v>2.8953823889591668</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <f>AVERAGE(B6:B7)</f>
-        <v>1.0003172062684076</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
         <f t="shared" ref="C8:D8" si="3">AVERAGE(C6:C7)</f>
         <v>2.9305909040190752</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <f t="shared" si="3"/>
         <v>2.9559871990529887</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
-        <f>(B6-B7)/2</f>
-        <v>2.5189544589605872E-2</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
         <f t="shared" ref="C9:D9" si="4">(C6-C7)/2</f>
         <v>5.4078033905484046E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <f t="shared" si="4"/>
         <v>6.0604810093822126E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4">
-        <f>B9/B8</f>
-        <v>2.5181556841927352E-2</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
         <f t="shared" ref="C10" si="5">C9/C8</f>
         <v>1.8452945387676004E-2</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f>D9/D8</f>
         <v>2.0502392606178445E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
         <f>B2/C2</f>
         <v>2.9302739238705087</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <f>C2/D2</f>
         <v>1.0086114101184069</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1">
         <f>C11*(1+C4)/(1-B4)</f>
         <v>2.9850397535597999</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <f>D11*(1+D4)/(1-C4)</f>
         <v>1.0225851166890751</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
         <f>C11*(1-C4)/(1+B4)</f>
         <v>2.8768702484256901</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <f>D11*(1-D4)/(1+C4)</f>
         <v>0.99480056360621372</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1">
         <f>AVERAGE(C12:C13)</f>
         <v>2.930955000992745</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <f>AVERAGE(D12:D13)</f>
         <v>1.0086928401476445</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1">
         <f>(C12-C13)/2</f>
         <v>5.4084752567054917E-2</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <f>(D12-D13)/2</f>
         <v>1.3892276541430715E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
         <f>C15/C14</f>
         <v>1.845294538767598E-2</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <f>D15/D14</f>
         <v>1.3772553931677827E-2</v>
       </c>

</xml_diff>

<commit_message>
feat: bigger hash table size on testing chore: experiment report changes
</commit_message>
<xml_diff>
--- a/results/bmark_combined.xlsx
+++ b/results/bmark_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\root\projects\hash_functions\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CF15FB-B096-45C0-9C3E-AF60C1FDB8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAD0658-B12E-4A7B-9C92-FB9FFD816500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4788" yWindow="1008" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>test_id</t>
   </si>
@@ -37,9 +37,6 @@
     <t>bmark_1</t>
   </si>
   <si>
-    <t>time_2</t>
-  </si>
-  <si>
     <t>avg</t>
   </si>
   <si>
@@ -83,6 +80,12 @@
   </si>
   <si>
     <t>abs. accel. rel. error</t>
+  </si>
+  <si>
+    <t>bmark_2</t>
+  </si>
+  <si>
+    <t>bmark_3</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +426,7 @@
     <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,455 +437,554 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4031250</v>
+        <v>703125</v>
       </c>
       <c r="C2">
-        <v>1375000</v>
+        <v>515625</v>
       </c>
       <c r="D2">
-        <v>1375000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E2">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4000000</v>
+        <v>718750</v>
       </c>
       <c r="C3">
-        <v>1375000</v>
+        <v>515625</v>
       </c>
       <c r="D3">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>515625</v>
+      </c>
+      <c r="E3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3984375</v>
+        <v>734375</v>
       </c>
       <c r="C4">
-        <v>1375000</v>
+        <v>531250</v>
       </c>
       <c r="D4">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E4">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4031250</v>
+        <v>765625</v>
       </c>
       <c r="C5">
-        <v>1375000</v>
+        <v>515625</v>
       </c>
       <c r="D5">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E5">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4000000</v>
+        <v>750000</v>
       </c>
       <c r="C6">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D6">
-        <v>1375000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E6">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4015625</v>
+        <v>703125</v>
       </c>
       <c r="C7">
-        <v>1359375</v>
+        <v>500000</v>
       </c>
       <c r="D7">
-        <v>1375000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>515625</v>
+      </c>
+      <c r="E7">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3968750</v>
+        <v>703125</v>
       </c>
       <c r="C8">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D8">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>531250</v>
+      </c>
+      <c r="E8">
+        <v>515625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4000000</v>
+        <v>703125</v>
       </c>
       <c r="C9">
-        <v>1375000</v>
+        <v>515625</v>
       </c>
       <c r="D9">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E9">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3984375</v>
+        <v>703125</v>
       </c>
       <c r="C10">
-        <v>1359375</v>
+        <v>484375</v>
       </c>
       <c r="D10">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>531250</v>
+      </c>
+      <c r="E10">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3984375</v>
+        <v>703125</v>
       </c>
       <c r="C11">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D11">
-        <v>1375000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>531250</v>
+      </c>
+      <c r="E11">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>3968750</v>
+        <v>718750</v>
       </c>
       <c r="C12">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D12">
-        <v>1375000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E12">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3984375</v>
+        <v>703125</v>
       </c>
       <c r="C13">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D13">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E13">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>3968750</v>
+        <v>718750</v>
       </c>
       <c r="C14">
-        <v>1359375</v>
+        <v>500000</v>
       </c>
       <c r="D14">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E14">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3968750</v>
+        <v>703125</v>
       </c>
       <c r="C15">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D15">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E15">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3968750</v>
+        <v>703125</v>
       </c>
       <c r="C16">
-        <v>1359375</v>
+        <v>484375</v>
       </c>
       <c r="D16">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E16">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>4000000</v>
+        <v>703125</v>
       </c>
       <c r="C17">
-        <v>1375000</v>
+        <v>515625</v>
       </c>
       <c r="D17">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E17">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>4046875</v>
+        <v>703125</v>
       </c>
       <c r="C18">
-        <v>1359375</v>
+        <v>484375</v>
       </c>
       <c r="D18">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E18">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>4125000</v>
+        <v>703125</v>
       </c>
       <c r="C19">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D19">
-        <v>1343750</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E19">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4031250</v>
+        <v>703125</v>
       </c>
       <c r="C20">
-        <v>1375000</v>
+        <v>484375</v>
       </c>
       <c r="D20">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E20">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>4046875</v>
+        <v>703125</v>
       </c>
       <c r="C21">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D21">
-        <v>1343750</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E21">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>4031250</v>
+        <v>703125</v>
       </c>
       <c r="C22">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D22">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E22">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>4000000</v>
+        <v>703125</v>
       </c>
       <c r="C23">
-        <v>1375000</v>
+        <v>484375</v>
       </c>
       <c r="D23">
-        <v>1375000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>468750</v>
+      </c>
+      <c r="E23">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>4000000</v>
+        <v>703125</v>
       </c>
       <c r="C24">
-        <v>1359375</v>
+        <v>500000</v>
       </c>
       <c r="D24">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E24">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>4015625</v>
+        <v>703125</v>
       </c>
       <c r="C25">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D25">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E25">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>4015625</v>
+        <v>703125</v>
       </c>
       <c r="C26">
-        <v>1375000</v>
+        <v>515625</v>
       </c>
       <c r="D26">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E26">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>4015625</v>
+        <v>703125</v>
       </c>
       <c r="C27">
-        <v>1375000</v>
+        <v>484375</v>
       </c>
       <c r="D27">
-        <v>1343750</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E27">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>4046875</v>
+        <v>703125</v>
       </c>
       <c r="C28">
-        <v>1375000</v>
+        <v>500000</v>
       </c>
       <c r="D28">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E28">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>4171875</v>
+        <v>718750</v>
       </c>
       <c r="C29">
-        <v>1375000</v>
+        <v>484375</v>
       </c>
       <c r="D29">
-        <v>1343750</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E29">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>4156250</v>
+        <v>718750</v>
       </c>
       <c r="C30">
-        <v>1390625</v>
+        <v>500000</v>
       </c>
       <c r="D30">
-        <v>1343750</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E30">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>4015625</v>
+        <v>703125</v>
       </c>
       <c r="C31">
-        <v>1375000</v>
+        <v>484375</v>
       </c>
       <c r="D31">
-        <v>1390625</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>484375</v>
+      </c>
+      <c r="E31">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>4062500</v>
+        <v>703125</v>
       </c>
       <c r="C32">
-        <v>1390625</v>
+        <v>500000</v>
       </c>
       <c r="D32">
-        <v>1359375</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500000</v>
+      </c>
+      <c r="E32">
+        <v>484375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>4062500</v>
+        <v>718750</v>
       </c>
       <c r="C33">
-        <v>1359375</v>
+        <v>500000</v>
       </c>
       <c r="D33">
-        <v>1359375</v>
+        <v>484375</v>
+      </c>
+      <c r="E33">
+        <v>484375</v>
       </c>
     </row>
   </sheetData>
@@ -892,10 +994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2184DC31-09BE-47B9-80E0-FCA191440139}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,7 +1006,7 @@
     <col min="2" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="str">
         <f>Results!B1</f>
         <v>bmark_0</v>
@@ -915,226 +1017,289 @@
       </c>
       <c r="D1" t="str">
         <f>Results!D1</f>
-        <v>time_2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>bmark_2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <f>AVERAGE(Results!B:B)/1000000</f>
-        <v>4.02197265625</v>
+        <v>0.71044921875</v>
       </c>
       <c r="C2" s="1">
         <f>AVERAGE(Results!C:C)/1000000</f>
-        <v>1.37255859375</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="1">
         <f>AVERAGE(Results!D:D)/1000000</f>
-        <v>1.36083984375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.4970703125</v>
+      </c>
+      <c r="E2" s="1">
+        <f>AVERAGE(Results!E:E)/1000000</f>
+        <v>0.49365234375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <f>_xlfn.STDEV.S(Results!B:B)/1000000</f>
-        <v>5.0647796882066408E-2</v>
+        <v>1.4841428617293475E-2</v>
       </c>
       <c r="C3" s="1">
         <f>_xlfn.STDEV.S(Results!C:C)/1000000</f>
-        <v>8.0452966859601242E-3</v>
+        <v>1.1906261906267861E-2</v>
       </c>
       <c r="D3" s="1">
         <f>_xlfn.STDEV.S(Results!D:D)/1000000</f>
-        <v>1.0766502448557674E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.5079959513587947E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <f>_xlfn.STDEV.S(Results!E:E)/1000000</f>
+        <v>8.7487173239000054E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <f>B3/B2</f>
-        <v>1.2592775041213063E-2</v>
+        <v>2.0890203304616519E-2</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:D4" si="0">C3/C2</f>
-        <v>5.8615324129656114E-3</v>
+        <f t="shared" ref="C4:E4" si="0">C3/C2</f>
+        <v>2.3812523812535721E-2</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>7.9116602133642334E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.0337678864271234E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7722426389067469E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:D5" si="1">$B2/C2</f>
-        <v>2.9302739238705087</v>
+        <f t="shared" ref="C5:E5" si="1">$B2/C2</f>
+        <v>1.4208984375</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>2.9555077143882311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.4292730844793713</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4391691394658754</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
         <f>C5*(1+$B4)/(1-C4)</f>
-        <v>2.9846689379245595</v>
+        <v>1.4859658929449548</v>
       </c>
       <c r="D6" s="1">
         <f>D5*(1+$B4)/(1-D4)</f>
-        <v>3.016592009146811</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.5047824979761375</v>
+      </c>
+      <c r="E6" s="1">
+        <f>E5*(1+$B4)/(1-E4)</f>
+        <v>1.4957418502165583</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <f t="shared" ref="C7:D7" si="2">C5*(1-$B4)/(1+C4)</f>
-        <v>2.8765128701135914</v>
+        <v>1.3588577477883541</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>2.8953823889591668</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3582103303349435</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7" si="3">E5*(1-$B4)/(1+E4)</f>
+        <v>1.3845667217458109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:D8" si="3">AVERAGE(C6:C7)</f>
-        <v>2.9305909040190752</v>
+        <f t="shared" ref="C8:D8" si="4">AVERAGE(C6:C7)</f>
+        <v>1.4224118203666545</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="3"/>
-        <v>2.9559871990529887</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1.4314964141555406</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ref="E8" si="5">AVERAGE(E6:E7)</f>
+        <v>1.4401542859811847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
-        <f t="shared" ref="C9:D9" si="4">(C6-C7)/2</f>
-        <v>5.4078033905484046E-2</v>
+        <f t="shared" ref="C9:D9" si="6">(C6-C7)/2</f>
+        <v>6.3554072578300369E-2</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="4"/>
-        <v>6.0604810093822126E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>7.3286083820596981E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" ref="E9" si="7">(E6-E7)/2</f>
+        <v>5.5587564235373699E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
-        <f t="shared" ref="C10" si="5">C9/C8</f>
-        <v>1.8452945387676004E-2</v>
+        <f t="shared" ref="C10" si="8">C9/C8</f>
+        <v>4.4680500870639607E-2</v>
       </c>
       <c r="D10" s="3">
         <f>D9/D8</f>
-        <v>2.0502392606178445E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.1195436534732394E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <f>E9/E8</f>
+        <v>3.8598339619912041E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
         <f>B2/C2</f>
-        <v>2.9302739238705087</v>
+        <v>1.4208984375</v>
       </c>
       <c r="D11" s="1">
         <f>C2/D2</f>
-        <v>1.0086114101184069</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.005893909626719</v>
+      </c>
+      <c r="E11" s="1">
+        <f>D2/E2</f>
+        <v>1.0069238377843719</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
         <f>C11*(1+C4)/(1-B4)</f>
-        <v>2.9850397535597999</v>
+        <v>1.4857716880048277</v>
       </c>
       <c r="D12" s="1">
         <f>D11*(1+D4)/(1-C4)</f>
-        <v>1.0225851166890751</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.0616919611345961</v>
+      </c>
+      <c r="E12" s="1">
+        <f>E11*(1+E4)/(1-D4)</f>
+        <v>1.0568307637019758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <f>C11*(1-C4)/(1+B4)</f>
-        <v>2.8768702484256901</v>
+        <v>1.3586801549587992</v>
       </c>
       <c r="D13" s="1">
         <f>D11*(1-D4)/(1+C4)</f>
-        <v>0.99480056360621372</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.95269143572571979</v>
+      </c>
+      <c r="E13" s="1">
+        <f>E11*(1-E4)/(1+D4)</f>
+        <v>0.95995587124416382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
         <f>AVERAGE(C12:C13)</f>
-        <v>2.930955000992745</v>
+        <v>1.4222259214818136</v>
       </c>
       <c r="D14" s="1">
         <f>AVERAGE(D12:D13)</f>
-        <v>1.0086928401476445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.0071916984301579</v>
+      </c>
+      <c r="E14" s="1">
+        <f>AVERAGE(E12:E13)</f>
+        <v>1.0083933174730699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
         <f>(C12-C13)/2</f>
-        <v>5.4084752567054917E-2</v>
+        <v>6.3545766523014247E-2</v>
       </c>
       <c r="D15" s="1">
         <f>(D12-D13)/2</f>
-        <v>1.3892276541430715E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.450026270443814E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <f>(E12-E13)/2</f>
+        <v>4.8437446228906E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
         <f>C15/C14</f>
-        <v>1.845294538767598E-2</v>
+        <v>4.468050087063951E-2</v>
       </c>
       <c r="D16" s="3">
         <f>D15/D14</f>
-        <v>1.3772553931677827E-2</v>
+        <v>5.4111111905890449E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <f>E15/E14</f>
+        <v>4.8034279273374468E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>